<commit_message>
Experiment running and giving ubermarks. Ubermarks not stimulus specific
</commit_message>
<xml_diff>
--- a/Psychopy/Music.xlsx
+++ b/Psychopy/Music.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uqjlarwo/Desktop/git/MusicAffectPsychophysiology2019/Experiment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uqjlarwo/Desktop/git/AlexithymiaMusicAffectPsychophysiology2019/Psychopy/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="4500" yWindow="1480" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>valence</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>30MonoWAV/30MonoT4.wav</t>
+  </si>
+  <si>
+    <t>marker</t>
   </si>
 </sst>
 </file>
@@ -426,18 +429,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -447,8 +450,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -458,8 +464,11 @@
       <c r="C2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -469,8 +478,11 @@
       <c r="C3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -480,8 +492,11 @@
       <c r="C4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -491,8 +506,11 @@
       <c r="C5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -502,8 +520,11 @@
       <c r="C6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -513,8 +534,11 @@
       <c r="C7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -524,8 +548,11 @@
       <c r="C8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -535,8 +562,11 @@
       <c r="C9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -546,8 +576,11 @@
       <c r="C10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -557,8 +590,11 @@
       <c r="C11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -568,8 +604,11 @@
       <c r="C12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -579,8 +618,11 @@
       <c r="C13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -590,8 +632,11 @@
       <c r="C14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -601,8 +646,11 @@
       <c r="C15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -612,8 +660,11 @@
       <c r="C16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -622,6 +673,9 @@
       </c>
       <c r="C17">
         <v>1</v>
+      </c>
+      <c r="D17">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>